<commit_message>
Updates to various interanl docs.
</commit_message>
<xml_diff>
--- a/docs/Splunk_REST_API.xlsx
+++ b/docs/Splunk_REST_API.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Refs" sheetId="4" r:id="rId2"/>
     <sheet name="Areas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1668,13 +1668,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D242" sqref="D242"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.140625" customWidth="1"/>
+    <col min="1" max="1" width="80.140625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
@@ -4792,12 +4792,12 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B19"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>